<commit_message>
bug fix sales order
</commit_message>
<xml_diff>
--- a/back/public/dealer/files/salesorder/excel/salesorder_2.xlsx
+++ b/back/public/dealer/files/salesorder/excel/salesorder_2.xlsx
@@ -11,97 +11,125 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
-  <si>
-    <t>Sales Order Number:</t>
-  </si>
-  <si>
-    <t>SS-01/101/03/JUL/2025</t>
-  </si>
-  <si>
-    <t>Date:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+  <si>
+    <t xml:space="preserve">PT. SUNWAY TREK MASINDO
+(A MEMBER OF THE SUNWAY GROUP)
+JL. KOSAMBI TIMUR NO.47
+KOMPLEKS PERGUDANGAN SENTRA KOSAMBI BLOK H1 NO.4 DADAP - TANGERANG
+TELP : 021-55595445 (Hunting)</t>
+  </si>
+  <si>
+    <t>SALES ORDER SUNFLEX STORE</t>
+  </si>
+  <si>
+    <t>SOLD TO:</t>
+  </si>
+  <si>
+    <t>CV Maju Abadi - jakartaa</t>
+  </si>
+  <si>
+    <t>SO NO</t>
+  </si>
+  <si>
+    <t>SS-01/101/08/JUL/2025</t>
+  </si>
+  <si>
+    <t>DELIVERED TO:</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
   <si>
     <t>7/3/2025</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
-    <t>MTR</t>
-  </si>
-  <si>
-    <t>Payment Term:</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Customer PO Number:</t>
-  </si>
-  <si>
-    <t>Delivery Order Number:</t>
-  </si>
-  <si>
-    <t>JDE Sales Order Number:</t>
-  </si>
-  <si>
-    <t>Sold To:</t>
-  </si>
-  <si>
-    <t>CV Maju Abadi - jakartaa</t>
-  </si>
-  <si>
-    <t>Delivered To:</t>
-  </si>
-  <si>
-    <t>No Address</t>
-  </si>
-  <si>
-    <t>Phone:</t>
-  </si>
-  <si>
-    <t>Fax:</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>PPN 11%</t>
-  </si>
-  <si>
-    <t>Final Price</t>
+    <t>PHONE:</t>
+  </si>
+  <si>
+    <t>PAYMENT TERM</t>
+  </si>
+  <si>
+    <t>FAX:</t>
+  </si>
+  <si>
+    <t>CUSTOMER PO NO</t>
+  </si>
+  <si>
+    <t>NO DO</t>
+  </si>
+  <si>
+    <t>NO SALES ORDER JDE</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PART NO</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>UNIT PRICE</t>
+  </si>
+  <si>
+    <t>PPN - 11%</t>
+  </si>
+  <si>
+    <t>UNIT SELL PRICE IDR</t>
+  </si>
+  <si>
+    <t>TOTAL PRICE</t>
   </si>
   <si>
     <t>AH300-0025</t>
   </si>
   <si>
-    <t>yesss</t>
+    <t>No Description</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
   <si>
     <t>AH300-0075</t>
   </si>
   <si>
-    <t>No Description</t>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>ORDERED BY</t>
+  </si>
+  <si>
+    <t>shobukid</t>
+  </si>
+  <si>
+    <t>CREDIT CONTROL</t>
+  </si>
+  <si>
+    <t>APPROVED BY</t>
+  </si>
+  <si>
+    <t>SALES PERSONNEL</t>
+  </si>
+  <si>
+    <t>superadminnn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -109,16 +137,45 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+    </font>
+    <font>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8EDF6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -133,13 +190,83 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,9 +294,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -187,6 +314,94 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -528,193 +743,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J19"/>
+  <sheetPr>
+    <tabColor rgb="FFB8CCE4"/>
+  </sheetPr>
+  <dimension ref="A1:I21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I3" s="1" t="s">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I5" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="1" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I10" s="1" t="s">
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="G12" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="I12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="10">
+        <v>30000</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3300</v>
+      </c>
+      <c r="H16" s="10">
+        <v>33300</v>
+      </c>
+      <c r="I16" s="10">
+        <v>33300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="10">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="10">
+        <v>114750</v>
+      </c>
+      <c r="G17" s="10">
+        <v>12623</v>
+      </c>
+      <c r="H17" s="10">
+        <v>127373</v>
+      </c>
+      <c r="I17" s="10">
+        <v>254746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12">
+        <v>288046</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>30000</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3300</v>
-      </c>
-      <c r="H18" s="1">
-        <v>33300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1">
-        <v>114750</v>
-      </c>
-      <c r="G19" s="1">
-        <v>12622.5</v>
-      </c>
-      <c r="H19" s="1">
-        <v>254745.00000000003</v>
-      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
+  <mergeCells count="12">
+    <mergeCell ref="C1:E5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>